<commit_message>
Fix Excel processor to handle merged cells for CPALMS URLs
</commit_message>
<xml_diff>
--- a/data/raw/BEST Math Extract.xlsx
+++ b/data/raw/BEST Math Extract.xlsx
@@ -5817,6 +5817,24 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5834,24 +5852,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="16" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -6606,8 +6606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D65300-00A7-466B-A236-C60FEC0F2948}">
   <dimension ref="A1:G712"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6621,26 +6621,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="46.9" customHeight="1" x14ac:dyDescent="1.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -6666,834 +6666,834 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="19"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="22"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="19"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="19"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="22"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="19"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="22"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="19"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="22"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="19"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="22"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="19"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="22"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="19"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="19"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="22"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="19"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="22"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="20"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="23"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="19"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="22"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="19"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="22"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="19"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="22"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="19"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="22"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="19"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="22"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="19"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="22"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="19"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="22"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="19"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="22"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="20"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="23"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="18" t="s">
+      <c r="D26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="19"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="22"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="19"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="22"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="19"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="22"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="19"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="22"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="19"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="22"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="19"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="22"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="19"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="22"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="19"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="22"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="20"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="23"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="18" t="s">
+      <c r="D36" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="19"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="22"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="19"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="22"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="19"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="22"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A40" s="19"/>
+      <c r="A40" s="16"/>
       <c r="B40" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" s="19"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="22"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="19"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="22"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="13"/>
     </row>
     <row r="43" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="19"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="22"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="13"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A44" s="19"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="22"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="13"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A45" s="19"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="22"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="13"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="20"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="23"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="14"/>
     </row>
     <row r="47" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="18" t="s">
+      <c r="D47" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="18" t="s">
+      <c r="F47" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" s="19"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="22"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="13"/>
     </row>
     <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A49" s="19"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="22"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A50" s="19"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="22"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="13"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A51" s="19"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="22"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="13"/>
     </row>
     <row r="52" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A52" s="19"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="22"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="13"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A53" s="19"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="22"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="13"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A54" s="19"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="22"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="13"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A55" s="19"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="22"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A56" s="19"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="22"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A57" s="20"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="9"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="23"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="18" t="s">
+      <c r="D58" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F58" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G58" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A59" s="19"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="4"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="22"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="13"/>
     </row>
     <row r="60" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A60" s="19"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="22"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="13"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A61" s="19"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="22"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="13"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A62" s="19"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="22"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="13"/>
     </row>
     <row r="63" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A63" s="19"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="22"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="13"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A64" s="19"/>
+      <c r="A64" s="16"/>
       <c r="B64" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="22"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="13"/>
     </row>
     <row r="65" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A65" s="19"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="22"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="13"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A66" s="19"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="22"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="13"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A67" s="20"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="9"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="23"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="14"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A68" s="18" t="s">
+      <c r="A68" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="18" t="s">
+      <c r="D68" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F68" s="18" t="s">
+      <c r="F68" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G68" s="21" t="s">
+      <c r="G68" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A69" s="19"/>
+      <c r="A69" s="16"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="22"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="13"/>
     </row>
     <row r="70" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A70" s="19"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C70" s="19"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="22"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="13"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A71" s="19"/>
+      <c r="A71" s="16"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="22"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="13"/>
     </row>
     <row r="72" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A72" s="19"/>
+      <c r="A72" s="16"/>
       <c r="B72" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="22"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="13"/>
     </row>
     <row r="73" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A73" s="19"/>
+      <c r="A73" s="16"/>
       <c r="B73" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="22"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="13"/>
     </row>
     <row r="74" spans="1:7" ht="39.4" x14ac:dyDescent="0.45">
-      <c r="A74" s="19"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="22"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="13"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A75" s="20"/>
+      <c r="A75" s="17"/>
       <c r="B75" s="9"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="23"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="14"/>
     </row>
     <row r="76" spans="1:7" ht="39.4" x14ac:dyDescent="0.45">
       <c r="A76" s="10" t="s">
@@ -16811,45 +16811,45 @@
       </c>
     </row>
     <row r="481" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A481" s="18" t="s">
+      <c r="A481" s="15" t="s">
         <v>1003</v>
       </c>
-      <c r="B481" s="18" t="s">
+      <c r="B481" s="15" t="s">
         <v>1004</v>
       </c>
-      <c r="C481" s="18" t="s">
+      <c r="C481" s="15" t="s">
         <v>994</v>
       </c>
-      <c r="D481" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E481" s="18">
-        <v>912</v>
-      </c>
-      <c r="F481" s="18" t="s">
+      <c r="D481" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E481" s="15">
+        <v>912</v>
+      </c>
+      <c r="F481" s="15" t="s">
         <v>929</v>
       </c>
-      <c r="G481" s="21" t="s">
+      <c r="G481" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A482" s="19"/>
-      <c r="B482" s="19"/>
-      <c r="C482" s="19"/>
-      <c r="D482" s="19"/>
-      <c r="E482" s="19"/>
-      <c r="F482" s="19"/>
-      <c r="G482" s="22"/>
+      <c r="A482" s="16"/>
+      <c r="B482" s="16"/>
+      <c r="C482" s="16"/>
+      <c r="D482" s="16"/>
+      <c r="E482" s="16"/>
+      <c r="F482" s="16"/>
+      <c r="G482" s="13"/>
     </row>
     <row r="483" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A483" s="20"/>
-      <c r="B483" s="20"/>
-      <c r="C483" s="20"/>
-      <c r="D483" s="20"/>
-      <c r="E483" s="20"/>
-      <c r="F483" s="20"/>
-      <c r="G483" s="23"/>
+      <c r="A483" s="17"/>
+      <c r="B483" s="17"/>
+      <c r="C483" s="17"/>
+      <c r="D483" s="17"/>
+      <c r="E483" s="17"/>
+      <c r="F483" s="17"/>
+      <c r="G483" s="14"/>
     </row>
     <row r="484" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A484" s="10" t="s">
@@ -22121,13 +22121,38 @@
   </sheetData>
   <autoFilter ref="A3:G712" xr:uid="{F1D65300-00A7-466B-A236-C60FEC0F2948}"/>
   <mergeCells count="51">
-    <mergeCell ref="G481:G483"/>
-    <mergeCell ref="A481:A483"/>
-    <mergeCell ref="B481:B483"/>
-    <mergeCell ref="C481:C483"/>
-    <mergeCell ref="D481:D483"/>
-    <mergeCell ref="E481:E483"/>
-    <mergeCell ref="F481:F483"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:A15"/>
+    <mergeCell ref="C4:C15"/>
+    <mergeCell ref="D4:D15"/>
+    <mergeCell ref="E4:E15"/>
+    <mergeCell ref="F4:F15"/>
+    <mergeCell ref="G4:G15"/>
+    <mergeCell ref="G26:G35"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="C16:C25"/>
+    <mergeCell ref="D16:D25"/>
+    <mergeCell ref="E16:E25"/>
+    <mergeCell ref="F16:F25"/>
+    <mergeCell ref="G16:G25"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="C26:C35"/>
+    <mergeCell ref="D26:D35"/>
+    <mergeCell ref="E26:E35"/>
+    <mergeCell ref="F26:F35"/>
+    <mergeCell ref="G47:G57"/>
+    <mergeCell ref="A36:A46"/>
+    <mergeCell ref="C36:C46"/>
+    <mergeCell ref="D36:D46"/>
+    <mergeCell ref="E36:E46"/>
+    <mergeCell ref="F36:F46"/>
+    <mergeCell ref="G36:G46"/>
+    <mergeCell ref="A47:A57"/>
+    <mergeCell ref="C47:C57"/>
+    <mergeCell ref="D47:D57"/>
+    <mergeCell ref="E47:E57"/>
+    <mergeCell ref="F47:F57"/>
     <mergeCell ref="G68:G75"/>
     <mergeCell ref="A58:A67"/>
     <mergeCell ref="C58:C67"/>
@@ -22140,38 +22165,13 @@
     <mergeCell ref="D68:D75"/>
     <mergeCell ref="E68:E75"/>
     <mergeCell ref="F68:F75"/>
-    <mergeCell ref="G47:G57"/>
-    <mergeCell ref="A36:A46"/>
-    <mergeCell ref="C36:C46"/>
-    <mergeCell ref="D36:D46"/>
-    <mergeCell ref="E36:E46"/>
-    <mergeCell ref="F36:F46"/>
-    <mergeCell ref="G36:G46"/>
-    <mergeCell ref="A47:A57"/>
-    <mergeCell ref="C47:C57"/>
-    <mergeCell ref="D47:D57"/>
-    <mergeCell ref="E47:E57"/>
-    <mergeCell ref="F47:F57"/>
-    <mergeCell ref="G26:G35"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="C16:C25"/>
-    <mergeCell ref="D16:D25"/>
-    <mergeCell ref="E16:E25"/>
-    <mergeCell ref="F16:F25"/>
-    <mergeCell ref="G16:G25"/>
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="C26:C35"/>
-    <mergeCell ref="D26:D35"/>
-    <mergeCell ref="E26:E35"/>
-    <mergeCell ref="F26:F35"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:A15"/>
-    <mergeCell ref="C4:C15"/>
-    <mergeCell ref="D4:D15"/>
-    <mergeCell ref="E4:E15"/>
-    <mergeCell ref="F4:F15"/>
-    <mergeCell ref="G4:G15"/>
+    <mergeCell ref="G481:G483"/>
+    <mergeCell ref="A481:A483"/>
+    <mergeCell ref="B481:B483"/>
+    <mergeCell ref="C481:C483"/>
+    <mergeCell ref="D481:D483"/>
+    <mergeCell ref="E481:E483"/>
+    <mergeCell ref="F481:F483"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.cpalms.org/" xr:uid="{366D235F-2F50-4071-BB84-A636DDF6C112}"/>

</xml_diff>